<commit_message>
Add limndiat to nemo pre-identified-missing list #807.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="896">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1696,10 +1696,16 @@
     <t xml:space="preserve"> P1 (1) growth_limitation_of_miscellaneous_phytoplankton_due_to_solar_irradiance : Phytoplankton are algae that grow where there is sufficient light to support photosynthesis. "Miscellaneous phytoplankton" are all those phytoplankton that are not diatoms, diazotrophs, calcareous phytoplankton, picophytoplankton or other separately named components of the phytoplankton population. The specification of a physical process by the phrase "due_to_" process means that the quantity named is a single term in a sum of terms which together compose the general quantity named by omitting the phrase. "Irradiance" means the power per unit area (called radiative flux in other standard names), the area being normal to the direction of flow of the radiant energy. Solar irradiance is essential to the photosynthesis reaction and its presence promotes the growth of phytoplankton populations. "Growth limitation due to solar irradiance" means the ratio of the growth rate of a species population in the environment (where the amount of sunlight reaching a location may be limited) to the theoretical growth rate if there were no such limit on solar irradiance. </t>
   </si>
   <si>
+    <t xml:space="preserve">limndiat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LDnutSFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1 (1) nitrogen_growth_limitation_of_diatoms : Diatoms are phytoplankton with an external skeleton made of silica. Phytoplankton are algae that grow where there is sufficient light to support photosynthesis. "Nitrogen growth limitation" means the ratio of the growth rate of a species population in the environment (where there is a finite availability of nitrogen) to the theoretical growth rate if there were no such limit on nitrogen availability.</t>
+  </si>
+  <si>
     <t xml:space="preserve">limndiaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LDnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve"> P1 (1) nitrogen_growth_limitation_of_diazotrophs : In ocean modelling, diazotrophs are phytoplankton of the phylum cyanobacteria distinct from other phytoplankton groups in their ability to fix nitrogen gas in addition to nitrate and ammonium. Phytoplankton are algae that grow where there is sufficient light to support photosynthesis. "Nitrogen growth limitation" means the ratio of the growth rate of a species population in the environment (where there is a finite availability of nitrogen) to the theoretical growth rate if there were no such limit on nitrogen availability. </t>
@@ -2801,28 +2807,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N298"/>
+  <dimension ref="A1:N299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M275" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M298" activeCellId="0" sqref="298:298"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="184:184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -2837,8 +2843,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="68.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="168.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="15" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6550,7 @@
         <v>561</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I185" s="0" t="s">
         <v>16</v>
@@ -6557,35 +6562,35 @@
         <v>1</v>
       </c>
       <c r="N185" s="0" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="H186" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="H186" s="0" t="s">
+      <c r="I186" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L186" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M186" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N186" s="0" t="s">
         <v>565</v>
-      </c>
-      <c r="I186" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L186" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M186" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N186" s="0" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="H187" s="0" t="s">
         <v>567</v>
-      </c>
-      <c r="H187" s="0" t="s">
-        <v>568</v>
       </c>
       <c r="I187" s="0" t="s">
         <v>16</v>
@@ -6597,15 +6602,15 @@
         <v>35</v>
       </c>
       <c r="N187" s="0" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="H188" s="0" t="s">
         <v>570</v>
-      </c>
-      <c r="H188" s="0" t="s">
-        <v>571</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>16</v>
@@ -6617,15 +6622,15 @@
         <v>35</v>
       </c>
       <c r="N188" s="0" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="s">
+        <v>572</v>
+      </c>
+      <c r="H189" s="0" t="s">
         <v>573</v>
-      </c>
-      <c r="H189" s="0" t="s">
-        <v>574</v>
       </c>
       <c r="I189" s="0" t="s">
         <v>16</v>
@@ -6637,7 +6642,7 @@
         <v>35</v>
       </c>
       <c r="N189" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6657,15 +6662,15 @@
         <v>35</v>
       </c>
       <c r="N190" s="0" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="H191" s="0" t="s">
         <v>578</v>
-      </c>
-      <c r="H191" s="0" t="s">
-        <v>579</v>
       </c>
       <c r="I191" s="0" t="s">
         <v>16</v>
@@ -6677,15 +6682,15 @@
         <v>35</v>
       </c>
       <c r="N191" s="0" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="H192" s="0" t="s">
         <v>581</v>
-      </c>
-      <c r="H192" s="0" t="s">
-        <v>582</v>
       </c>
       <c r="I192" s="0" t="s">
         <v>16</v>
@@ -6697,7 +6702,7 @@
         <v>35</v>
       </c>
       <c r="N192" s="0" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6714,18 +6719,18 @@
         <v>369</v>
       </c>
       <c r="M193" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N193" s="0" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="H194" s="0" t="s">
         <v>586</v>
-      </c>
-      <c r="H194" s="0" t="s">
-        <v>587</v>
       </c>
       <c r="I194" s="0" t="s">
         <v>16</v>
@@ -6737,15 +6742,15 @@
         <v>413</v>
       </c>
       <c r="N194" s="0" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="H195" s="0" t="s">
         <v>589</v>
-      </c>
-      <c r="H195" s="0" t="s">
-        <v>590</v>
       </c>
       <c r="I195" s="0" t="s">
         <v>16</v>
@@ -6757,35 +6762,35 @@
         <v>413</v>
       </c>
       <c r="N195" s="0" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="H196" s="0" t="s">
         <v>592</v>
       </c>
-      <c r="H196" s="0" t="s">
+      <c r="I196" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L196" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M196" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="N196" s="0" t="s">
         <v>593</v>
-      </c>
-      <c r="I196" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L196" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M196" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N196" s="0" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="H197" s="0" t="s">
         <v>595</v>
-      </c>
-      <c r="H197" s="0" t="s">
-        <v>596</v>
       </c>
       <c r="I197" s="0" t="s">
         <v>16</v>
@@ -6797,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="N197" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6813,19 +6818,19 @@
       <c r="L198" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M198" s="0" t="s">
-        <v>35</v>
+      <c r="M198" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N198" s="0" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="H199" s="0" t="s">
         <v>600</v>
-      </c>
-      <c r="H199" s="0" t="s">
-        <v>601</v>
       </c>
       <c r="I199" s="0" t="s">
         <v>16</v>
@@ -6837,7 +6842,7 @@
         <v>35</v>
       </c>
       <c r="N199" s="0" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6857,15 +6862,15 @@
         <v>35</v>
       </c>
       <c r="N200" s="0" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="H201" s="0" t="s">
         <v>605</v>
-      </c>
-      <c r="H201" s="0" t="s">
-        <v>606</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>16</v>
@@ -6877,15 +6882,15 @@
         <v>35</v>
       </c>
       <c r="N201" s="0" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="H202" s="0" t="s">
         <v>608</v>
-      </c>
-      <c r="H202" s="0" t="s">
-        <v>609</v>
       </c>
       <c r="I202" s="0" t="s">
         <v>16</v>
@@ -6897,15 +6902,15 @@
         <v>35</v>
       </c>
       <c r="N202" s="0" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="H203" s="0" t="s">
         <v>611</v>
-      </c>
-      <c r="H203" s="0" t="s">
-        <v>612</v>
       </c>
       <c r="I203" s="0" t="s">
         <v>16</v>
@@ -6917,7 +6922,7 @@
         <v>35</v>
       </c>
       <c r="N203" s="0" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6925,7 +6930,7 @@
         <v>613</v>
       </c>
       <c r="H204" s="0" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
       <c r="I204" s="0" t="s">
         <v>16</v>
@@ -6937,7 +6942,7 @@
         <v>35</v>
       </c>
       <c r="N204" s="0" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6945,7 +6950,7 @@
         <v>615</v>
       </c>
       <c r="H205" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I205" s="0" t="s">
         <v>16</v>
@@ -6965,7 +6970,7 @@
         <v>617</v>
       </c>
       <c r="H206" s="0" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
       <c r="I206" s="0" t="s">
         <v>16</v>
@@ -6977,15 +6982,15 @@
         <v>35</v>
       </c>
       <c r="N206" s="0" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="H207" s="0" t="s">
         <v>620</v>
-      </c>
-      <c r="H207" s="0" t="s">
-        <v>621</v>
       </c>
       <c r="I207" s="0" t="s">
         <v>16</v>
@@ -6997,7 +7002,7 @@
         <v>35</v>
       </c>
       <c r="N207" s="0" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7014,38 +7019,38 @@
         <v>369</v>
       </c>
       <c r="M208" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N208" s="0" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="H209" s="0" t="s">
         <v>625</v>
       </c>
-      <c r="H209" s="0" t="s">
+      <c r="I209" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L209" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M209" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="N209" s="0" t="s">
         <v>626</v>
-      </c>
-      <c r="I209" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L209" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M209" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N209" s="0" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="H210" s="0" t="s">
         <v>628</v>
-      </c>
-      <c r="H210" s="0" t="s">
-        <v>629</v>
       </c>
       <c r="I210" s="0" t="s">
         <v>16</v>
@@ -7057,7 +7062,7 @@
         <v>35</v>
       </c>
       <c r="N210" s="0" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7074,18 +7079,18 @@
         <v>369</v>
       </c>
       <c r="M211" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N211" s="0" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="H212" s="0" t="s">
         <v>633</v>
-      </c>
-      <c r="H212" s="0" t="s">
-        <v>634</v>
       </c>
       <c r="I212" s="0" t="s">
         <v>16</v>
@@ -7097,15 +7102,15 @@
         <v>413</v>
       </c>
       <c r="N212" s="0" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="H213" s="0" t="s">
         <v>636</v>
-      </c>
-      <c r="H213" s="0" t="s">
-        <v>637</v>
       </c>
       <c r="I213" s="0" t="s">
         <v>16</v>
@@ -7117,15 +7122,15 @@
         <v>413</v>
       </c>
       <c r="N213" s="0" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="H214" s="0" t="s">
         <v>639</v>
-      </c>
-      <c r="H214" s="0" t="s">
-        <v>640</v>
       </c>
       <c r="I214" s="0" t="s">
         <v>16</v>
@@ -7137,7 +7142,7 @@
         <v>413</v>
       </c>
       <c r="N214" s="0" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7157,35 +7162,35 @@
         <v>413</v>
       </c>
       <c r="N215" s="0" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="H216" s="0" t="s">
         <v>644</v>
       </c>
-      <c r="H216" s="0" t="s">
+      <c r="I216" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L216" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M216" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="N216" s="0" t="s">
         <v>645</v>
-      </c>
-      <c r="I216" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L216" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M216" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N216" s="0" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="H217" s="0" t="s">
         <v>647</v>
-      </c>
-      <c r="H217" s="0" t="s">
-        <v>648</v>
       </c>
       <c r="I217" s="0" t="s">
         <v>16</v>
@@ -7197,7 +7202,7 @@
         <v>35</v>
       </c>
       <c r="N217" s="0" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,38 +7219,38 @@
         <v>369</v>
       </c>
       <c r="M218" s="0" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="N218" s="0" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="H219" s="0" t="s">
         <v>652</v>
       </c>
-      <c r="H219" s="0" t="s">
+      <c r="I219" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L219" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M219" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="N219" s="0" t="s">
         <v>653</v>
-      </c>
-      <c r="I219" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L219" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M219" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N219" s="0" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="H220" s="0" t="s">
         <v>655</v>
-      </c>
-      <c r="H220" s="0" t="s">
-        <v>653</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>16</v>
@@ -7265,7 +7270,7 @@
         <v>657</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>16</v>
@@ -7277,7 +7282,7 @@
         <v>35</v>
       </c>
       <c r="N221" s="0" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7285,7 +7290,7 @@
         <v>659</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>16</v>
@@ -7297,15 +7302,15 @@
         <v>35</v>
       </c>
       <c r="N222" s="0" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="H223" s="0" t="s">
         <v>660</v>
-      </c>
-      <c r="H223" s="0" t="s">
-        <v>661</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>16</v>
@@ -7317,15 +7322,15 @@
         <v>35</v>
       </c>
       <c r="N223" s="0" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="H224" s="0" t="s">
         <v>663</v>
-      </c>
-      <c r="H224" s="0" t="s">
-        <v>664</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>16</v>
@@ -7337,15 +7342,15 @@
         <v>35</v>
       </c>
       <c r="N224" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="H225" s="0" t="s">
         <v>666</v>
-      </c>
-      <c r="H225" s="0" t="s">
-        <v>667</v>
       </c>
       <c r="I225" s="0" t="s">
         <v>16</v>
@@ -7357,15 +7362,15 @@
         <v>35</v>
       </c>
       <c r="N225" s="0" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="H226" s="0" t="s">
         <v>669</v>
-      </c>
-      <c r="H226" s="0" t="s">
-        <v>670</v>
       </c>
       <c r="I226" s="0" t="s">
         <v>16</v>
@@ -7377,36 +7382,36 @@
         <v>35</v>
       </c>
       <c r="N226" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="H227" s="0" t="s">
         <v>672</v>
       </c>
-      <c r="H227" s="0" t="s">
+      <c r="I227" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L227" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M227" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N227" s="0" t="s">
         <v>673</v>
-      </c>
-      <c r="I227" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L227" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M227" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N227" s="0" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="H228" s="0" t="s">
         <v>675</v>
       </c>
-      <c r="H228" s="0" t="s">
-        <v>667</v>
-      </c>
       <c r="I228" s="0" t="s">
         <v>16</v>
       </c>
@@ -7414,7 +7419,7 @@
         <v>369</v>
       </c>
       <c r="M228" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="N228" s="0" t="s">
         <v>676</v>
@@ -7425,7 +7430,7 @@
         <v>677</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>16</v>
@@ -7445,1385 +7450,1405 @@
         <v>679</v>
       </c>
       <c r="H230" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="I230" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L230" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M230" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N230" s="0" t="s">
         <v>680</v>
-      </c>
-      <c r="I230" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L230" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M230" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="N230" s="0" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="H231" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="I231" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L231" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M231" s="0" t="s">
         <v>684</v>
       </c>
-      <c r="H231" s="0" t="s">
+      <c r="N231" s="0" t="s">
         <v>685</v>
-      </c>
-      <c r="I231" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L231" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M231" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="N231" s="0" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="H232" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="H232" s="0" t="s">
+      <c r="I232" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L232" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M232" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="N232" s="0" t="s">
         <v>688</v>
-      </c>
-      <c r="I232" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L232" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M232" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="N232" s="0" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="H233" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="I233" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L233" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M233" s="0" t="s">
         <v>691</v>
       </c>
-      <c r="H233" s="0" t="s">
+      <c r="N233" s="0" t="s">
         <v>692</v>
-      </c>
-      <c r="I233" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L233" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M233" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="N233" s="0" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="H234" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="H234" s="0" t="s">
+      <c r="I234" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L234" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M234" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="N234" s="0" t="s">
         <v>695</v>
-      </c>
-      <c r="I234" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L234" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M234" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="N234" s="0" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="H235" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="I235" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L235" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M235" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="H235" s="0" t="s">
+      <c r="N235" s="0" t="s">
         <v>699</v>
-      </c>
-      <c r="I235" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L235" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M235" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="N235" s="0" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="H236" s="0" t="s">
         <v>701</v>
       </c>
-      <c r="H236" s="0" t="s">
+      <c r="I236" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L236" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M236" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="N236" s="0" t="s">
         <v>702</v>
-      </c>
-      <c r="I236" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L236" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M236" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="N236" s="0" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="H237" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="I237" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L237" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M237" s="0" t="s">
         <v>705</v>
       </c>
-      <c r="H237" s="0" t="s">
+      <c r="N237" s="0" t="s">
         <v>706</v>
-      </c>
-      <c r="I237" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L237" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M237" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="N237" s="0" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="H238" s="0" t="s">
         <v>708</v>
       </c>
-      <c r="H238" s="0" t="s">
+      <c r="I238" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L238" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M238" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="N238" s="0" t="s">
         <v>709</v>
-      </c>
-      <c r="I238" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L238" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M238" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="N238" s="0" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="H239" s="0" t="s">
         <v>711</v>
       </c>
-      <c r="H239" s="0" t="s">
+      <c r="I239" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L239" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M239" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="N239" s="0" t="s">
         <v>712</v>
-      </c>
-      <c r="I239" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L239" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M239" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="N239" s="0" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="H240" s="0" t="s">
         <v>714</v>
       </c>
-      <c r="H240" s="0" t="s">
-        <v>715</v>
-      </c>
       <c r="I240" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L240" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M240" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N240" s="0" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="H241" s="0" t="s">
         <v>717</v>
       </c>
-      <c r="H241" s="0" t="s">
-        <v>718</v>
-      </c>
       <c r="I241" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L241" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M241" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N241" s="0" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="H242" s="0" t="s">
         <v>720</v>
       </c>
-      <c r="H242" s="0" t="s">
-        <v>721</v>
-      </c>
       <c r="I242" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L242" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M242" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N242" s="0" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="H243" s="0" t="s">
         <v>723</v>
       </c>
-      <c r="H243" s="0" t="s">
-        <v>724</v>
-      </c>
       <c r="I243" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L243" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M243" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N243" s="0" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="H244" s="0" t="s">
         <v>726</v>
       </c>
-      <c r="H244" s="0" t="s">
-        <v>727</v>
-      </c>
       <c r="I244" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L244" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M244" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N244" s="0" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="s">
+        <v>728</v>
+      </c>
+      <c r="H245" s="0" t="s">
         <v>729</v>
       </c>
-      <c r="H245" s="0" t="s">
-        <v>730</v>
-      </c>
       <c r="I245" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L245" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M245" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N245" s="0" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="s">
+        <v>731</v>
+      </c>
+      <c r="H246" s="0" t="s">
         <v>732</v>
       </c>
-      <c r="H246" s="0" t="s">
-        <v>733</v>
-      </c>
       <c r="I246" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L246" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M246" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N246" s="0" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="s">
+        <v>734</v>
+      </c>
+      <c r="H247" s="0" t="s">
         <v>735</v>
       </c>
-      <c r="H247" s="0" t="s">
+      <c r="I247" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L247" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M247" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N247" s="0" t="s">
         <v>736</v>
-      </c>
-      <c r="I247" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L247" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M247" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="N247" s="0" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="H248" s="0" t="s">
         <v>738</v>
       </c>
-      <c r="H248" s="0" t="s">
-        <v>739</v>
-      </c>
       <c r="I248" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L248" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M248" s="0" t="s">
         <v>162</v>
       </c>
       <c r="N248" s="0" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="H249" s="0" t="s">
         <v>741</v>
       </c>
-      <c r="H249" s="0" t="s">
+      <c r="I249" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L249" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M249" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="N249" s="0" t="s">
         <v>742</v>
-      </c>
-      <c r="I249" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L249" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M249" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="N249" s="0" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="H250" s="0" t="s">
         <v>744</v>
       </c>
-      <c r="H250" s="0" t="s">
+      <c r="I250" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L250" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M250" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="N250" s="0" t="s">
         <v>745</v>
-      </c>
-      <c r="I250" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L250" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M250" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="N250" s="0" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="H251" s="0" t="s">
         <v>747</v>
       </c>
-      <c r="H251" s="0" t="s">
+      <c r="I251" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L251" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M251" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="N251" s="0" t="s">
         <v>748</v>
-      </c>
-      <c r="I251" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L251" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M251" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N251" s="0" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="s">
+        <v>749</v>
+      </c>
+      <c r="H252" s="0" t="s">
         <v>750</v>
       </c>
-      <c r="H252" s="0" t="s">
+      <c r="I252" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L252" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M252" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N252" s="0" t="s">
         <v>751</v>
-      </c>
-      <c r="I252" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L252" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M252" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="N252" s="0" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="H253" s="0" t="s">
         <v>753</v>
       </c>
-      <c r="H253" s="0" t="s">
-        <v>754</v>
-      </c>
       <c r="I253" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L253" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M253" s="0" t="s">
         <v>69</v>
       </c>
       <c r="N253" s="0" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="s">
+        <v>755</v>
+      </c>
+      <c r="H254" s="0" t="s">
         <v>756</v>
       </c>
-      <c r="H254" s="0" t="s">
+      <c r="I254" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L254" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M254" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N254" s="0" t="s">
         <v>757</v>
-      </c>
-      <c r="I254" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L254" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M254" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="N254" s="0" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="s">
+        <v>758</v>
+      </c>
+      <c r="H255" s="0" t="s">
         <v>759</v>
       </c>
-      <c r="H255" s="0" t="s">
-        <v>760</v>
-      </c>
       <c r="I255" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L255" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M255" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N255" s="0" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="H256" s="0" t="s">
         <v>762</v>
       </c>
-      <c r="H256" s="0" t="s">
+      <c r="I256" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L256" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M256" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N256" s="0" t="s">
         <v>763</v>
-      </c>
-      <c r="I256" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L256" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M256" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="N256" s="0" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="H257" s="0" t="s">
         <v>765</v>
       </c>
-      <c r="H257" s="0" t="s">
-        <v>766</v>
-      </c>
       <c r="I257" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L257" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M257" s="0" t="s">
         <v>69</v>
       </c>
       <c r="N257" s="0" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="s">
+        <v>767</v>
+      </c>
+      <c r="H258" s="0" t="s">
         <v>768</v>
       </c>
-      <c r="H258" s="0" t="s">
+      <c r="I258" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L258" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M258" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N258" s="0" t="s">
         <v>769</v>
-      </c>
-      <c r="I258" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L258" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M258" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="N258" s="0" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="s">
+        <v>770</v>
+      </c>
+      <c r="H259" s="0" t="s">
         <v>771</v>
       </c>
-      <c r="H259" s="0" t="s">
-        <v>772</v>
-      </c>
       <c r="I259" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L259" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M259" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N259" s="0" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="H260" s="0" t="s">
         <v>774</v>
       </c>
-      <c r="H260" s="0" t="s">
-        <v>775</v>
-      </c>
       <c r="I260" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L260" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M260" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N260" s="0" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="H261" s="0" t="s">
         <v>777</v>
       </c>
-      <c r="H261" s="0" t="s">
-        <v>778</v>
-      </c>
       <c r="I261" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L261" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M261" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N261" s="0" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="H262" s="0" t="s">
         <v>780</v>
       </c>
-      <c r="H262" s="0" t="s">
-        <v>781</v>
-      </c>
       <c r="I262" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L262" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M262" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N262" s="0" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="H263" s="0" t="s">
         <v>783</v>
       </c>
-      <c r="H263" s="0" t="s">
-        <v>784</v>
-      </c>
       <c r="I263" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L263" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M263" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N263" s="0" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="H264" s="0" t="s">
         <v>786</v>
       </c>
-      <c r="H264" s="0" t="s">
+      <c r="I264" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L264" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M264" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N264" s="0" t="s">
         <v>787</v>
-      </c>
-      <c r="I264" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L264" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M264" s="0" t="s">
-        <v>788</v>
-      </c>
-      <c r="N264" s="0" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="0" t="s">
+        <v>788</v>
+      </c>
+      <c r="H265" s="0" t="s">
+        <v>789</v>
+      </c>
+      <c r="I265" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L265" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M265" s="0" t="s">
         <v>790</v>
       </c>
-      <c r="H265" s="0" t="s">
+      <c r="N265" s="0" t="s">
         <v>791</v>
-      </c>
-      <c r="I265" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L265" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M265" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="N265" s="0" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="H266" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="H266" s="0" t="s">
+      <c r="I266" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L266" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M266" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="N266" s="0" t="s">
         <v>794</v>
-      </c>
-      <c r="I266" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L266" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M266" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N266" s="0" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="H267" s="0" t="s">
         <v>796</v>
       </c>
-      <c r="H267" s="0" t="s">
-        <v>797</v>
-      </c>
       <c r="I267" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L267" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M267" s="0" t="s">
         <v>42</v>
       </c>
       <c r="N267" s="0" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="s">
+        <v>798</v>
+      </c>
+      <c r="H268" s="0" t="s">
         <v>799</v>
       </c>
-      <c r="H268" s="0" t="s">
+      <c r="I268" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L268" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M268" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N268" s="0" t="s">
         <v>800</v>
-      </c>
-      <c r="I268" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L268" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M268" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="N268" s="0" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="H269" s="0" t="s">
         <v>802</v>
       </c>
-      <c r="H269" s="0" t="s">
+      <c r="I269" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L269" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M269" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="N269" s="0" t="s">
         <v>803</v>
-      </c>
-      <c r="I269" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L269" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M269" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="N269" s="0" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="H270" s="0" t="s">
         <v>805</v>
       </c>
-      <c r="H270" s="0" t="s">
+      <c r="I270" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L270" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M270" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="N270" s="0" t="s">
         <v>806</v>
-      </c>
-      <c r="I270" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L270" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M270" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="N270" s="0" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="0" t="s">
+        <v>807</v>
+      </c>
+      <c r="H271" s="0" t="s">
         <v>808</v>
       </c>
-      <c r="H271" s="0" t="s">
+      <c r="I271" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L271" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M271" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N271" s="0" t="s">
         <v>809</v>
-      </c>
-      <c r="I271" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L271" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M271" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="N271" s="0" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="H272" s="0" t="s">
         <v>811</v>
       </c>
-      <c r="H272" s="0" t="s">
+      <c r="I272" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L272" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M272" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="N272" s="0" t="s">
         <v>812</v>
-      </c>
-      <c r="I272" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L272" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M272" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="N272" s="0" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="s">
+        <v>813</v>
+      </c>
+      <c r="H273" s="0" t="s">
         <v>814</v>
       </c>
-      <c r="H273" s="0" t="s">
+      <c r="I273" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L273" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M273" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="N273" s="0" t="s">
         <v>815</v>
-      </c>
-      <c r="I273" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L273" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M273" s="0" t="s">
-        <v>788</v>
-      </c>
-      <c r="N273" s="0" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="H274" s="0" t="s">
         <v>817</v>
       </c>
-      <c r="H274" s="0" t="s">
+      <c r="I274" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L274" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M274" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="N274" s="0" t="s">
         <v>818</v>
-      </c>
-      <c r="I274" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L274" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M274" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="N274" s="0" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="H275" s="0" t="s">
         <v>820</v>
       </c>
-      <c r="H275" s="0" t="s">
+      <c r="I275" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L275" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M275" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="N275" s="0" t="s">
         <v>821</v>
-      </c>
-      <c r="I275" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L275" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M275" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N275" s="0" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="H276" s="0" t="s">
         <v>823</v>
       </c>
-      <c r="H276" s="0" t="s">
+      <c r="I276" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L276" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M276" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N276" s="0" t="s">
         <v>824</v>
-      </c>
-      <c r="I276" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L276" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M276" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="N276" s="0" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="H277" s="0" t="s">
         <v>826</v>
       </c>
-      <c r="H277" s="0" t="s">
+      <c r="I277" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L277" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M277" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="N277" s="0" t="s">
         <v>827</v>
-      </c>
-      <c r="I277" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L277" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M277" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="N277" s="0" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="H278" s="0" t="s">
         <v>829</v>
       </c>
-      <c r="H278" s="0" t="s">
+      <c r="I278" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L278" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M278" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="N278" s="0" t="s">
         <v>830</v>
-      </c>
-      <c r="I278" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L278" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M278" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="N278" s="0" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="H279" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="H279" s="0" t="s">
+      <c r="I279" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L279" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M279" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="N279" s="0" t="s">
         <v>833</v>
-      </c>
-      <c r="I279" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L279" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M279" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="N279" s="0" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="H280" s="0" t="s">
         <v>835</v>
       </c>
-      <c r="H280" s="0" t="s">
-        <v>836</v>
-      </c>
       <c r="I280" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L280" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M280" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N280" s="0" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H281" s="0" t="s">
         <v>838</v>
       </c>
-      <c r="H281" s="0" t="s">
-        <v>839</v>
-      </c>
       <c r="I281" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L281" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M281" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N281" s="0" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="H282" s="0" t="s">
         <v>841</v>
       </c>
-      <c r="H282" s="0" t="s">
-        <v>842</v>
-      </c>
       <c r="I282" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L282" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M282" s="0" t="s">
         <v>280</v>
       </c>
       <c r="N282" s="0" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="H283" s="0" t="s">
         <v>844</v>
       </c>
-      <c r="H283" s="0" t="s">
+      <c r="I283" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L283" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M283" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N283" s="0" t="s">
         <v>845</v>
-      </c>
-      <c r="I283" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L283" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M283" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="N283" s="0" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="H284" s="0" t="s">
+        <v>847</v>
+      </c>
+      <c r="I284" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L284" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M284" s="0" t="s">
         <v>848</v>
       </c>
-      <c r="H284" s="0" t="s">
+      <c r="N284" s="0" t="s">
         <v>849</v>
-      </c>
-      <c r="I284" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L284" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M284" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="N284" s="0" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="H285" s="0" t="s">
         <v>851</v>
       </c>
-      <c r="H285" s="0" t="s">
+      <c r="I285" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L285" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M285" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="N285" s="0" t="s">
         <v>852</v>
-      </c>
-      <c r="I285" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L285" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M285" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="N285" s="0" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="H286" s="0" t="s">
         <v>854</v>
       </c>
-      <c r="H286" s="0" t="s">
+      <c r="I286" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L286" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M286" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="N286" s="0" t="s">
         <v>855</v>
-      </c>
-      <c r="I286" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L286" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M286" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N286" s="0" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="H287" s="0" t="s">
         <v>857</v>
       </c>
-      <c r="H287" s="0" t="s">
+      <c r="I287" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L287" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M287" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N287" s="0" t="s">
         <v>858</v>
-      </c>
-      <c r="I287" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L287" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M287" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N287" s="0" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="H288" s="0" t="s">
         <v>860</v>
       </c>
-      <c r="H288" s="0" t="s">
+      <c r="I288" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L288" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M288" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N288" s="0" t="s">
         <v>861</v>
-      </c>
-      <c r="I288" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L288" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M288" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="N288" s="0" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="H289" s="0" t="s">
         <v>863</v>
       </c>
-      <c r="H289" s="0" t="s">
-        <v>864</v>
-      </c>
       <c r="I289" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L289" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M289" s="0" t="s">
         <v>330</v>
       </c>
       <c r="N289" s="0" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="H290" s="0" t="s">
         <v>866</v>
       </c>
-      <c r="H290" s="0" t="s">
+      <c r="I290" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L290" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M290" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="N290" s="0" t="s">
         <v>867</v>
-      </c>
-      <c r="I290" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L290" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M290" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N290" s="0" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="H291" s="0" t="s">
         <v>869</v>
       </c>
-      <c r="H291" s="0" t="s">
+      <c r="I291" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L291" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M291" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N291" s="0" t="s">
         <v>870</v>
-      </c>
-      <c r="I291" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L291" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M291" s="0" t="s">
-        <v>871</v>
-      </c>
-      <c r="N291" s="0" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="H292" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="I292" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L292" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M292" s="0" t="s">
         <v>873</v>
       </c>
-      <c r="H292" s="0" t="s">
+      <c r="N292" s="0" t="s">
         <v>874</v>
-      </c>
-      <c r="I292" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L292" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M292" s="0" t="s">
-        <v>871</v>
-      </c>
-      <c r="N292" s="0" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="s">
+        <v>875</v>
+      </c>
+      <c r="H293" s="0" t="s">
         <v>876</v>
       </c>
-      <c r="H293" s="0" t="s">
+      <c r="I293" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L293" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M293" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="N293" s="0" t="s">
         <v>877</v>
-      </c>
-      <c r="I293" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L293" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M293" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="N293" s="0" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="H294" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="H294" s="0" t="s">
-        <v>880</v>
-      </c>
       <c r="I294" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L294" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M294" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N294" s="0" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="s">
+        <v>881</v>
+      </c>
+      <c r="H295" s="0" t="s">
         <v>882</v>
       </c>
-      <c r="H295" s="0" t="s">
-        <v>883</v>
-      </c>
       <c r="I295" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L295" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M295" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N295" s="0" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="s">
+        <v>884</v>
+      </c>
+      <c r="H296" s="0" t="s">
         <v>885</v>
       </c>
-      <c r="H296" s="0" t="s">
-        <v>886</v>
-      </c>
       <c r="I296" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L296" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M296" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N296" s="0" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="H297" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="H297" s="0" t="s">
-        <v>889</v>
-      </c>
       <c r="I297" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L297" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="M297" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N297" s="0" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="H298" s="0" t="s">
         <v>891</v>
       </c>
-      <c r="H298" s="0" t="s">
+      <c r="I298" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L298" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M298" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N298" s="0" t="s">
         <v>892</v>
       </c>
-      <c r="I298" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L298" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M298" s="0" t="s">
+    </row>
+    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B299" s="0" t="s">
+        <v>893</v>
+      </c>
+      <c r="H299" s="0" t="s">
+        <v>894</v>
+      </c>
+      <c r="I299" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L299" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="M299" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="N298" s="0" t="s">
-        <v>893</v>
+      <c r="N299" s="0" t="s">
+        <v>895</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add intpoc & siflsaltbot to the pre nemo identified missing #811 #813.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="902">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1603,10 +1603,19 @@
     <t xml:space="preserve">intpcalcite</t>
   </si>
   <si>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P1 (mol m-2 s-1) tendency_of_ocean_mole_content_of_calcite_expressed_as_carbon_due_to_biological_production : Vertically integrated calcite production </t>
+  </si>
+  <si>
+    <t xml:space="preserve">intpoc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPCAL</t>
   </si>
   <si>
-    <t xml:space="preserve"> P1 (mol m-2 s-1) tendency_of_ocean_mole_content_of_calcite_expressed_as_carbon_due_to_biological_production : Vertically integrated calcite production </t>
+    <t xml:space="preserve"> P2 (kg m-2) ocean_mass_content_of_particulate_organic_matter_expressed_as_carbon : Vertically integrated POC</t>
   </si>
   <si>
     <t xml:space="preserve">intpn2</t>
@@ -1967,6 +1976,15 @@
   </si>
   <si>
     <t xml:space="preserve"> P1 (mol m-3) mole_concentration_of_dissolved_inorganic_silicon_in_sea_water : Mole concentration means number of moles per unit volume, also called "molarity", and is used in the construction "mole_concentration_of_X_in_Y", where X is a material constituent of Y. A chemical or biological species denoted by X may be described by a single term such as "nitrogen" or a phrase such as "nox_expressed_as_nitrogen". "Dissolved inorganic silicon" means the sum of all inorganic silicon in solution (including silicic acid and its first dissociated anion SiO(OH)3-). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">siflsaltbot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: sfx_mv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P2 (kg m-2 s-1) siflsaltbot : Total flux of salt from water into sea ice divided by grid-cell area; salt flux is upward (negative) during ice growth when salt is embedded into the ice and downward (positive) during melt when salt from sea ice is again released to the oceanP2 (kg m-2 s-1) siflsaltbot : Total flux of salt from water into sea ice divided by grid-cell area; salt flux is upward (negative) during ice growth when salt is embedded into the ice and downward (positive) during melt when salt from sea ice is again released to the ocean</t>
   </si>
   <si>
     <t xml:space="preserve">sios</t>
@@ -2718,7 +2736,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2748,6 +2766,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2792,7 +2816,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2802,6 +2826,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2822,13 +2850,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N299"/>
+  <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="184:184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I173" activeCellId="0" sqref="I173:I174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -6339,7 +6367,7 @@
         <v>369</v>
       </c>
       <c r="M174" s="0" t="s">
-        <v>448</v>
+        <v>154</v>
       </c>
       <c r="N174" s="0" t="s">
         <v>531</v>
@@ -6370,7 +6398,7 @@
         <v>535</v>
       </c>
       <c r="H176" s="0" t="s">
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="I176" s="0" t="s">
         <v>16</v>
@@ -6382,15 +6410,15 @@
         <v>448</v>
       </c>
       <c r="N176" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="I177" s="0" t="s">
         <v>16</v>
@@ -6458,8 +6486,8 @@
       <c r="L180" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M180" s="0" t="n">
-        <v>1</v>
+      <c r="M180" s="0" t="s">
+        <v>448</v>
       </c>
       <c r="N180" s="0" t="s">
         <v>548</v>
@@ -6550,7 +6578,7 @@
         <v>561</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="I185" s="0" t="s">
         <v>16</v>
@@ -6562,15 +6590,15 @@
         <v>1</v>
       </c>
       <c r="N185" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I186" s="0" t="s">
         <v>16</v>
@@ -6598,8 +6626,8 @@
       <c r="L187" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M187" s="0" t="s">
-        <v>35</v>
+      <c r="M187" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N187" s="0" t="s">
         <v>568</v>
@@ -6662,15 +6690,15 @@
         <v>35</v>
       </c>
       <c r="N190" s="0" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H191" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I191" s="0" t="s">
         <v>16</v>
@@ -6682,7 +6710,7 @@
         <v>35</v>
       </c>
       <c r="N191" s="0" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6722,15 +6750,15 @@
         <v>35</v>
       </c>
       <c r="N193" s="0" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="H194" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="I194" s="0" t="s">
         <v>16</v>
@@ -6739,10 +6767,10 @@
         <v>369</v>
       </c>
       <c r="M194" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N194" s="0" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6798,8 +6826,8 @@
       <c r="L197" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M197" s="0" t="n">
-        <v>1</v>
+      <c r="M197" s="0" t="s">
+        <v>413</v>
       </c>
       <c r="N197" s="0" t="s">
         <v>596</v>
@@ -6822,27 +6850,27 @@
         <v>1</v>
       </c>
       <c r="N198" s="0" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="H199" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="I199" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L199" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M199" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N199" s="0" t="s">
         <v>599</v>
-      </c>
-      <c r="H199" s="0" t="s">
-        <v>600</v>
-      </c>
-      <c r="I199" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L199" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M199" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N199" s="0" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6862,15 +6890,15 @@
         <v>35</v>
       </c>
       <c r="N200" s="0" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>16</v>
@@ -6882,7 +6910,7 @@
         <v>35</v>
       </c>
       <c r="N201" s="0" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6942,15 +6970,15 @@
         <v>35</v>
       </c>
       <c r="N204" s="0" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H205" s="0" t="s">
-        <v>600</v>
+        <v>617</v>
       </c>
       <c r="I205" s="0" t="s">
         <v>16</v>
@@ -6962,12 +6990,12 @@
         <v>35</v>
       </c>
       <c r="N205" s="0" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="H206" s="0" t="s">
         <v>603</v>
@@ -6982,15 +7010,15 @@
         <v>35</v>
       </c>
       <c r="N206" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="I207" s="0" t="s">
         <v>16</v>
@@ -7022,27 +7050,27 @@
         <v>35</v>
       </c>
       <c r="N208" s="0" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="H209" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="I209" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L209" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M209" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N209" s="0" t="s">
         <v>624</v>
-      </c>
-      <c r="H209" s="0" t="s">
-        <v>625</v>
-      </c>
-      <c r="I209" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L209" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M209" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="N209" s="0" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7059,7 +7087,7 @@
         <v>369</v>
       </c>
       <c r="M210" s="0" t="s">
-        <v>35</v>
+        <v>413</v>
       </c>
       <c r="N210" s="0" t="s">
         <v>629</v>
@@ -7082,27 +7110,27 @@
         <v>35</v>
       </c>
       <c r="N211" s="0" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="s">
+        <v>633</v>
+      </c>
+      <c r="H212" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="I212" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L212" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M212" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N212" s="0" t="s">
         <v>632</v>
-      </c>
-      <c r="H212" s="0" t="s">
-        <v>633</v>
-      </c>
-      <c r="I212" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L212" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="M212" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="N212" s="0" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7162,15 +7190,15 @@
         <v>413</v>
       </c>
       <c r="N215" s="0" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="H216" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="I216" s="0" t="s">
         <v>16</v>
@@ -7182,7 +7210,7 @@
         <v>413</v>
       </c>
       <c r="N216" s="0" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7199,7 +7227,7 @@
         <v>369</v>
       </c>
       <c r="M217" s="0" t="s">
-        <v>35</v>
+        <v>413</v>
       </c>
       <c r="N217" s="0" t="s">
         <v>648</v>
@@ -7222,35 +7250,35 @@
         <v>35</v>
       </c>
       <c r="N218" s="0" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H219" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="I219" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="L219" s="0" t="s">
+      <c r="L219" s="3" t="s">
         <v>369</v>
       </c>
       <c r="M219" s="0" t="s">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="N219" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>16</v>
@@ -7262,7 +7290,7 @@
         <v>35</v>
       </c>
       <c r="N220" s="0" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7270,7 +7298,7 @@
         <v>657</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>16</v>
@@ -7279,18 +7307,18 @@
         <v>369</v>
       </c>
       <c r="M221" s="0" t="s">
-        <v>35</v>
+        <v>219</v>
       </c>
       <c r="N221" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>16</v>
@@ -7302,15 +7330,15 @@
         <v>35</v>
       </c>
       <c r="N222" s="0" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="H223" s="0" t="s">
         <v>661</v>
-      </c>
-      <c r="H223" s="0" t="s">
-        <v>660</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>16</v>
@@ -7322,15 +7350,15 @@
         <v>35</v>
       </c>
       <c r="N223" s="0" t="s">
-        <v>656</v>
+        <v>664</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>16</v>
@@ -7347,7 +7375,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="H225" s="0" t="s">
         <v>666</v>
@@ -7362,7 +7390,7 @@
         <v>35</v>
       </c>
       <c r="N225" s="0" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7419,7 +7447,7 @@
         <v>369</v>
       </c>
       <c r="M228" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N228" s="0" t="s">
         <v>676</v>
@@ -7430,7 +7458,7 @@
         <v>677</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>16</v>
@@ -7442,15 +7470,15 @@
         <v>35</v>
       </c>
       <c r="N229" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="H230" s="0" t="s">
-        <v>672</v>
+        <v>681</v>
       </c>
       <c r="I230" s="0" t="s">
         <v>16</v>
@@ -7459,187 +7487,187 @@
         <v>369</v>
       </c>
       <c r="M230" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="N230" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="H231" s="0" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="I231" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L231" s="0" t="s">
-        <v>683</v>
+        <v>369</v>
       </c>
       <c r="M231" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N231" s="0" t="s">
         <v>684</v>
-      </c>
-      <c r="N231" s="0" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="H232" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="I232" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L232" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="M232" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N232" s="0" t="s">
         <v>686</v>
-      </c>
-      <c r="H232" s="0" t="s">
-        <v>687</v>
-      </c>
-      <c r="I232" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L232" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M232" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="N232" s="0" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="H233" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="I233" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L233" s="0" t="s">
         <v>689</v>
       </c>
-      <c r="H233" s="0" t="s">
+      <c r="M233" s="0" t="s">
         <v>690</v>
       </c>
-      <c r="I233" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L233" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M233" s="0" t="s">
+      <c r="N233" s="0" t="s">
         <v>691</v>
-      </c>
-      <c r="N233" s="0" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="H234" s="0" t="s">
         <v>693</v>
       </c>
-      <c r="H234" s="0" t="s">
+      <c r="I234" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L234" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M234" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="N234" s="0" t="s">
         <v>694</v>
-      </c>
-      <c r="I234" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L234" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M234" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="N234" s="0" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="H235" s="0" t="s">
         <v>696</v>
       </c>
-      <c r="H235" s="0" t="s">
+      <c r="I235" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L235" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M235" s="0" t="s">
         <v>697</v>
       </c>
-      <c r="I235" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L235" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M235" s="0" t="s">
+      <c r="N235" s="0" t="s">
         <v>698</v>
-      </c>
-      <c r="N235" s="0" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="H236" s="0" t="s">
         <v>700</v>
       </c>
-      <c r="H236" s="0" t="s">
+      <c r="I236" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L236" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M236" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="N236" s="0" t="s">
         <v>701</v>
-      </c>
-      <c r="I236" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L236" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M236" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="N236" s="0" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="H237" s="0" t="s">
         <v>703</v>
       </c>
-      <c r="H237" s="0" t="s">
+      <c r="I237" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L237" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M237" s="0" t="s">
         <v>704</v>
       </c>
-      <c r="I237" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L237" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M237" s="0" t="s">
+      <c r="N237" s="0" t="s">
         <v>705</v>
-      </c>
-      <c r="N237" s="0" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="H238" s="0" t="s">
         <v>707</v>
       </c>
-      <c r="H238" s="0" t="s">
+      <c r="I238" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L238" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M238" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="N238" s="0" t="s">
         <v>708</v>
-      </c>
-      <c r="I238" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L238" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M238" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="N238" s="0" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="H239" s="0" t="s">
         <v>710</v>
       </c>
-      <c r="H239" s="0" t="s">
+      <c r="I239" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L239" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M239" s="0" t="s">
         <v>711</v>
-      </c>
-      <c r="I239" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L239" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M239" s="0" t="s">
-        <v>705</v>
       </c>
       <c r="N239" s="0" t="s">
         <v>712</v>
@@ -7656,10 +7684,10 @@
         <v>16</v>
       </c>
       <c r="L240" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M240" s="0" t="s">
-        <v>76</v>
+        <v>711</v>
       </c>
       <c r="N240" s="0" t="s">
         <v>715</v>
@@ -7676,10 +7704,10 @@
         <v>16</v>
       </c>
       <c r="L241" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M241" s="0" t="s">
-        <v>76</v>
+        <v>711</v>
       </c>
       <c r="N241" s="0" t="s">
         <v>718</v>
@@ -7696,7 +7724,7 @@
         <v>16</v>
       </c>
       <c r="L242" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M242" s="0" t="s">
         <v>76</v>
@@ -7716,7 +7744,7 @@
         <v>16</v>
       </c>
       <c r="L243" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M243" s="0" t="s">
         <v>76</v>
@@ -7736,7 +7764,7 @@
         <v>16</v>
       </c>
       <c r="L244" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M244" s="0" t="s">
         <v>76</v>
@@ -7756,7 +7784,7 @@
         <v>16</v>
       </c>
       <c r="L245" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M245" s="0" t="s">
         <v>76</v>
@@ -7776,7 +7804,7 @@
         <v>16</v>
       </c>
       <c r="L246" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M246" s="0" t="s">
         <v>76</v>
@@ -7796,7 +7824,7 @@
         <v>16</v>
       </c>
       <c r="L247" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M247" s="0" t="s">
         <v>76</v>
@@ -7816,10 +7844,10 @@
         <v>16</v>
       </c>
       <c r="L248" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M248" s="0" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="N248" s="0" t="s">
         <v>739</v>
@@ -7836,10 +7864,10 @@
         <v>16</v>
       </c>
       <c r="L249" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M249" s="0" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="N249" s="0" t="s">
         <v>742</v>
@@ -7856,10 +7884,10 @@
         <v>16</v>
       </c>
       <c r="L250" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M250" s="0" t="s">
-        <v>691</v>
+        <v>162</v>
       </c>
       <c r="N250" s="0" t="s">
         <v>745</v>
@@ -7876,10 +7904,10 @@
         <v>16</v>
       </c>
       <c r="L251" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M251" s="0" t="s">
-        <v>691</v>
+        <v>162</v>
       </c>
       <c r="N251" s="0" t="s">
         <v>748</v>
@@ -7896,10 +7924,10 @@
         <v>16</v>
       </c>
       <c r="L252" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M252" s="0" t="s">
-        <v>42</v>
+        <v>697</v>
       </c>
       <c r="N252" s="0" t="s">
         <v>751</v>
@@ -7916,10 +7944,10 @@
         <v>16</v>
       </c>
       <c r="L253" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M253" s="0" t="s">
-        <v>69</v>
+        <v>697</v>
       </c>
       <c r="N253" s="0" t="s">
         <v>754</v>
@@ -7936,10 +7964,10 @@
         <v>16</v>
       </c>
       <c r="L254" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M254" s="0" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="N254" s="0" t="s">
         <v>757</v>
@@ -7956,10 +7984,10 @@
         <v>16</v>
       </c>
       <c r="L255" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M255" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N255" s="0" t="s">
         <v>760</v>
@@ -7976,10 +8004,10 @@
         <v>16</v>
       </c>
       <c r="L256" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M256" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N256" s="0" t="s">
         <v>763</v>
@@ -7996,10 +8024,10 @@
         <v>16</v>
       </c>
       <c r="L257" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M257" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N257" s="0" t="s">
         <v>766</v>
@@ -8016,10 +8044,10 @@
         <v>16</v>
       </c>
       <c r="L258" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M258" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N258" s="0" t="s">
         <v>769</v>
@@ -8036,10 +8064,10 @@
         <v>16</v>
       </c>
       <c r="L259" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M259" s="0" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="N259" s="0" t="s">
         <v>772</v>
@@ -8056,10 +8084,10 @@
         <v>16</v>
       </c>
       <c r="L260" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M260" s="0" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="N260" s="0" t="s">
         <v>775</v>
@@ -8076,7 +8104,7 @@
         <v>16</v>
       </c>
       <c r="L261" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M261" s="0" t="s">
         <v>280</v>
@@ -8096,7 +8124,7 @@
         <v>16</v>
       </c>
       <c r="L262" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M262" s="0" t="s">
         <v>280</v>
@@ -8116,7 +8144,7 @@
         <v>16</v>
       </c>
       <c r="L263" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M263" s="0" t="s">
         <v>280</v>
@@ -8136,7 +8164,7 @@
         <v>16</v>
       </c>
       <c r="L264" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M264" s="0" t="s">
         <v>280</v>
@@ -8156,50 +8184,50 @@
         <v>16</v>
       </c>
       <c r="L265" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M265" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N265" s="0" t="s">
         <v>790</v>
-      </c>
-      <c r="N265" s="0" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="s">
+        <v>791</v>
+      </c>
+      <c r="H266" s="0" t="s">
         <v>792</v>
       </c>
-      <c r="H266" s="0" t="s">
+      <c r="I266" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L266" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M266" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N266" s="0" t="s">
         <v>793</v>
-      </c>
-      <c r="I266" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L266" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M266" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="N266" s="0" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="H267" s="0" t="s">
         <v>795</v>
       </c>
-      <c r="H267" s="0" t="s">
+      <c r="I267" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L267" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M267" s="0" t="s">
         <v>796</v>
-      </c>
-      <c r="I267" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L267" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M267" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="N267" s="0" t="s">
         <v>797</v>
@@ -8216,10 +8244,10 @@
         <v>16</v>
       </c>
       <c r="L268" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M268" s="0" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="N268" s="0" t="s">
         <v>800</v>
@@ -8236,10 +8264,10 @@
         <v>16</v>
       </c>
       <c r="L269" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M269" s="0" t="s">
-        <v>154</v>
+        <v>42</v>
       </c>
       <c r="N269" s="0" t="s">
         <v>803</v>
@@ -8256,10 +8284,10 @@
         <v>16</v>
       </c>
       <c r="L270" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M270" s="0" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="N270" s="0" t="s">
         <v>806</v>
@@ -8276,10 +8304,10 @@
         <v>16</v>
       </c>
       <c r="L271" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M271" s="0" t="n">
-        <v>0.001</v>
+        <v>689</v>
+      </c>
+      <c r="M271" s="0" t="s">
+        <v>154</v>
       </c>
       <c r="N271" s="0" t="s">
         <v>809</v>
@@ -8296,10 +8324,10 @@
         <v>16</v>
       </c>
       <c r="L272" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M272" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="N272" s="0" t="s">
         <v>812</v>
@@ -8316,10 +8344,10 @@
         <v>16</v>
       </c>
       <c r="L273" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M273" s="0" t="s">
-        <v>705</v>
+        <v>689</v>
+      </c>
+      <c r="M273" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="N273" s="0" t="s">
         <v>815</v>
@@ -8336,10 +8364,10 @@
         <v>16</v>
       </c>
       <c r="L274" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M274" s="0" t="s">
-        <v>790</v>
+        <v>154</v>
       </c>
       <c r="N274" s="0" t="s">
         <v>818</v>
@@ -8356,10 +8384,10 @@
         <v>16</v>
       </c>
       <c r="L275" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M275" s="0" t="s">
-        <v>154</v>
+        <v>711</v>
       </c>
       <c r="N275" s="0" t="s">
         <v>821</v>
@@ -8376,10 +8404,10 @@
         <v>16</v>
       </c>
       <c r="L276" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M276" s="0" t="s">
-        <v>42</v>
+        <v>796</v>
       </c>
       <c r="N276" s="0" t="s">
         <v>824</v>
@@ -8396,10 +8424,10 @@
         <v>16</v>
       </c>
       <c r="L277" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M277" s="0" t="s">
-        <v>330</v>
+        <v>154</v>
       </c>
       <c r="N277" s="0" t="s">
         <v>827</v>
@@ -8416,10 +8444,10 @@
         <v>16</v>
       </c>
       <c r="L278" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M278" s="0" t="s">
-        <v>698</v>
+        <v>42</v>
       </c>
       <c r="N278" s="0" t="s">
         <v>830</v>
@@ -8436,10 +8464,10 @@
         <v>16</v>
       </c>
       <c r="L279" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M279" s="0" t="s">
-        <v>698</v>
+        <v>330</v>
       </c>
       <c r="N279" s="0" t="s">
         <v>833</v>
@@ -8456,10 +8484,10 @@
         <v>16</v>
       </c>
       <c r="L280" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M280" s="0" t="s">
-        <v>280</v>
+        <v>704</v>
       </c>
       <c r="N280" s="0" t="s">
         <v>836</v>
@@ -8476,10 +8504,10 @@
         <v>16</v>
       </c>
       <c r="L281" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M281" s="0" t="s">
-        <v>280</v>
+        <v>704</v>
       </c>
       <c r="N281" s="0" t="s">
         <v>839</v>
@@ -8496,7 +8524,7 @@
         <v>16</v>
       </c>
       <c r="L282" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M282" s="0" t="s">
         <v>280</v>
@@ -8516,7 +8544,7 @@
         <v>16</v>
       </c>
       <c r="L283" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M283" s="0" t="s">
         <v>280</v>
@@ -8536,50 +8564,50 @@
         <v>16</v>
       </c>
       <c r="L284" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M284" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N284" s="0" t="s">
         <v>848</v>
-      </c>
-      <c r="N284" s="0" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
+        <v>849</v>
+      </c>
+      <c r="H285" s="0" t="s">
         <v>850</v>
       </c>
-      <c r="H285" s="0" t="s">
+      <c r="I285" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L285" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M285" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="N285" s="0" t="s">
         <v>851</v>
-      </c>
-      <c r="I285" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L285" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M285" s="0" t="s">
-        <v>848</v>
-      </c>
-      <c r="N285" s="0" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="H286" s="0" t="s">
         <v>853</v>
       </c>
-      <c r="H286" s="0" t="s">
+      <c r="I286" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L286" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M286" s="0" t="s">
         <v>854</v>
-      </c>
-      <c r="I286" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L286" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M286" s="0" t="s">
-        <v>848</v>
       </c>
       <c r="N286" s="0" t="s">
         <v>855</v>
@@ -8596,10 +8624,10 @@
         <v>16</v>
       </c>
       <c r="L287" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M287" s="0" t="s">
-        <v>42</v>
+        <v>854</v>
       </c>
       <c r="N287" s="0" t="s">
         <v>858</v>
@@ -8616,10 +8644,10 @@
         <v>16</v>
       </c>
       <c r="L288" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M288" s="0" t="n">
-        <v>1</v>
+        <v>689</v>
+      </c>
+      <c r="M288" s="0" t="s">
+        <v>854</v>
       </c>
       <c r="N288" s="0" t="s">
         <v>861</v>
@@ -8636,10 +8664,10 @@
         <v>16</v>
       </c>
       <c r="L289" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M289" s="0" t="s">
-        <v>330</v>
+        <v>42</v>
       </c>
       <c r="N289" s="0" t="s">
         <v>864</v>
@@ -8656,10 +8684,10 @@
         <v>16</v>
       </c>
       <c r="L290" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M290" s="0" t="s">
-        <v>330</v>
+        <v>689</v>
+      </c>
+      <c r="M290" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N290" s="0" t="s">
         <v>867</v>
@@ -8676,10 +8704,10 @@
         <v>16</v>
       </c>
       <c r="L291" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M291" s="0" t="s">
-        <v>42</v>
+        <v>330</v>
       </c>
       <c r="N291" s="0" t="s">
         <v>870</v>
@@ -8696,50 +8724,50 @@
         <v>16</v>
       </c>
       <c r="L292" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M292" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="N292" s="0" t="s">
         <v>873</v>
-      </c>
-      <c r="N292" s="0" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="H293" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="H293" s="0" t="s">
+      <c r="I293" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L293" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M293" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N293" s="0" t="s">
         <v>876</v>
-      </c>
-      <c r="I293" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L293" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M293" s="0" t="s">
-        <v>873</v>
-      </c>
-      <c r="N293" s="0" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="H294" s="0" t="s">
         <v>878</v>
       </c>
-      <c r="H294" s="0" t="s">
+      <c r="I294" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L294" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M294" s="0" t="s">
         <v>879</v>
-      </c>
-      <c r="I294" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L294" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="M294" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="N294" s="0" t="s">
         <v>880</v>
@@ -8756,10 +8784,10 @@
         <v>16</v>
       </c>
       <c r="L295" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M295" s="0" t="s">
-        <v>76</v>
+        <v>879</v>
       </c>
       <c r="N295" s="0" t="s">
         <v>883</v>
@@ -8776,7 +8804,7 @@
         <v>16</v>
       </c>
       <c r="L296" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M296" s="0" t="s">
         <v>76</v>
@@ -8796,7 +8824,7 @@
         <v>16</v>
       </c>
       <c r="L297" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M297" s="0" t="s">
         <v>76</v>
@@ -8816,7 +8844,7 @@
         <v>16</v>
       </c>
       <c r="L298" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M298" s="0" t="s">
         <v>76</v>
@@ -8836,13 +8864,53 @@
         <v>16</v>
       </c>
       <c r="L299" s="0" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M299" s="0" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="N299" s="0" t="s">
         <v>895</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B300" s="0" t="s">
+        <v>896</v>
+      </c>
+      <c r="H300" s="0" t="s">
+        <v>897</v>
+      </c>
+      <c r="I300" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L300" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M300" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N300" s="0" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B301" s="0" t="s">
+        <v>899</v>
+      </c>
+      <c r="H301" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="I301" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L301" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="M301" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="N301" s="0" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct siflsaltbot in nemo-ony pre identified missing: seaIce var instead of ocnBgchem #811.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -1981,7 +1981,10 @@
     <t xml:space="preserve">siflsaltbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: sfx_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: sfx_mv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seaIce</t>
   </si>
   <si>
     <t xml:space="preserve"> P2 (kg m-2 s-1) siflsaltbot : Total flux of salt from water into sea ice divided by grid-cell area; salt flux is upward (negative) during ice growth when salt is embedded into the ice and downward (positive) during melt when salt from sea ice is again released to the oceanP2 (kg m-2 s-1) siflsaltbot : Total flux of salt from water into sea ice divided by grid-cell area; salt flux is upward (negative) during ice growth when salt is embedded into the ice and downward (positive) during melt when salt from sea ice is again released to the ocean</t>
@@ -2087,9 +2090,6 @@
   </si>
   <si>
     <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: iceage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seaIce</t>
   </si>
   <si>
     <t xml:space="preserve">s</t>
@@ -2852,8 +2852,8 @@
   </sheetPr>
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I173" activeCellId="0" sqref="I173:I174"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="219:219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7264,21 +7264,21 @@
         <v>16</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>369</v>
+        <v>654</v>
       </c>
       <c r="M219" s="0" t="s">
         <v>76</v>
       </c>
       <c r="N219" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>16</v>
@@ -7295,10 +7295,10 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>16</v>
@@ -7310,15 +7310,15 @@
         <v>219</v>
       </c>
       <c r="N221" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>16</v>
@@ -7330,15 +7330,15 @@
         <v>35</v>
       </c>
       <c r="N222" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="H223" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>16</v>
@@ -7350,15 +7350,15 @@
         <v>35</v>
       </c>
       <c r="N223" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>16</v>
@@ -7370,15 +7370,15 @@
         <v>35</v>
       </c>
       <c r="N224" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="H225" s="0" t="s">
         <v>667</v>
-      </c>
-      <c r="H225" s="0" t="s">
-        <v>666</v>
       </c>
       <c r="I225" s="0" t="s">
         <v>16</v>
@@ -7390,15 +7390,15 @@
         <v>35</v>
       </c>
       <c r="N225" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H226" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I226" s="0" t="s">
         <v>16</v>
@@ -7410,15 +7410,15 @@
         <v>35</v>
       </c>
       <c r="N226" s="0" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="H227" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I227" s="0" t="s">
         <v>16</v>
@@ -7430,15 +7430,15 @@
         <v>35</v>
       </c>
       <c r="N227" s="0" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H228" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="I228" s="0" t="s">
         <v>16</v>
@@ -7450,15 +7450,15 @@
         <v>35</v>
       </c>
       <c r="N228" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>16</v>
@@ -7470,15 +7470,15 @@
         <v>35</v>
       </c>
       <c r="N229" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H230" s="0" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="I230" s="0" t="s">
         <v>16</v>
@@ -7490,15 +7490,15 @@
         <v>42</v>
       </c>
       <c r="N230" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="H231" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="I231" s="0" t="s">
         <v>16</v>
@@ -7510,15 +7510,15 @@
         <v>35</v>
       </c>
       <c r="N231" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H232" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="I232" s="0" t="s">
         <v>16</v>
@@ -7530,21 +7530,21 @@
         <v>35</v>
       </c>
       <c r="N232" s="0" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="H233" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="I233" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L233" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M233" s="0" t="s">
         <v>690</v>
@@ -7564,7 +7564,7 @@
         <v>16</v>
       </c>
       <c r="L234" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M234" s="0" t="s">
         <v>46</v>
@@ -7584,7 +7584,7 @@
         <v>16</v>
       </c>
       <c r="L235" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M235" s="0" t="s">
         <v>697</v>
@@ -7604,7 +7604,7 @@
         <v>16</v>
       </c>
       <c r="L236" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M236" s="0" t="s">
         <v>697</v>
@@ -7624,7 +7624,7 @@
         <v>16</v>
       </c>
       <c r="L237" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M237" s="0" t="s">
         <v>704</v>
@@ -7644,7 +7644,7 @@
         <v>16</v>
       </c>
       <c r="L238" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M238" s="0" t="s">
         <v>240</v>
@@ -7664,7 +7664,7 @@
         <v>16</v>
       </c>
       <c r="L239" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M239" s="0" t="s">
         <v>711</v>
@@ -7684,7 +7684,7 @@
         <v>16</v>
       </c>
       <c r="L240" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M240" s="0" t="s">
         <v>711</v>
@@ -7704,7 +7704,7 @@
         <v>16</v>
       </c>
       <c r="L241" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M241" s="0" t="s">
         <v>711</v>
@@ -7724,7 +7724,7 @@
         <v>16</v>
       </c>
       <c r="L242" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M242" s="0" t="s">
         <v>76</v>
@@ -7744,7 +7744,7 @@
         <v>16</v>
       </c>
       <c r="L243" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M243" s="0" t="s">
         <v>76</v>
@@ -7764,7 +7764,7 @@
         <v>16</v>
       </c>
       <c r="L244" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M244" s="0" t="s">
         <v>76</v>
@@ -7784,7 +7784,7 @@
         <v>16</v>
       </c>
       <c r="L245" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M245" s="0" t="s">
         <v>76</v>
@@ -7804,7 +7804,7 @@
         <v>16</v>
       </c>
       <c r="L246" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M246" s="0" t="s">
         <v>76</v>
@@ -7824,7 +7824,7 @@
         <v>16</v>
       </c>
       <c r="L247" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M247" s="0" t="s">
         <v>76</v>
@@ -7844,7 +7844,7 @@
         <v>16</v>
       </c>
       <c r="L248" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M248" s="0" t="s">
         <v>76</v>
@@ -7864,7 +7864,7 @@
         <v>16</v>
       </c>
       <c r="L249" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M249" s="0" t="s">
         <v>76</v>
@@ -7884,7 +7884,7 @@
         <v>16</v>
       </c>
       <c r="L250" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M250" s="0" t="s">
         <v>162</v>
@@ -7904,7 +7904,7 @@
         <v>16</v>
       </c>
       <c r="L251" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M251" s="0" t="s">
         <v>162</v>
@@ -7924,7 +7924,7 @@
         <v>16</v>
       </c>
       <c r="L252" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M252" s="0" t="s">
         <v>697</v>
@@ -7944,7 +7944,7 @@
         <v>16</v>
       </c>
       <c r="L253" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M253" s="0" t="s">
         <v>697</v>
@@ -7964,7 +7964,7 @@
         <v>16</v>
       </c>
       <c r="L254" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M254" s="0" t="s">
         <v>42</v>
@@ -7984,7 +7984,7 @@
         <v>16</v>
       </c>
       <c r="L255" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M255" s="0" t="s">
         <v>69</v>
@@ -8004,7 +8004,7 @@
         <v>16</v>
       </c>
       <c r="L256" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M256" s="0" t="s">
         <v>69</v>
@@ -8024,7 +8024,7 @@
         <v>16</v>
       </c>
       <c r="L257" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M257" s="0" t="s">
         <v>76</v>
@@ -8044,7 +8044,7 @@
         <v>16</v>
       </c>
       <c r="L258" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M258" s="0" t="s">
         <v>76</v>
@@ -8064,7 +8064,7 @@
         <v>16</v>
       </c>
       <c r="L259" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M259" s="0" t="s">
         <v>69</v>
@@ -8084,7 +8084,7 @@
         <v>16</v>
       </c>
       <c r="L260" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M260" s="0" t="s">
         <v>69</v>
@@ -8104,7 +8104,7 @@
         <v>16</v>
       </c>
       <c r="L261" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M261" s="0" t="s">
         <v>280</v>
@@ -8124,7 +8124,7 @@
         <v>16</v>
       </c>
       <c r="L262" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M262" s="0" t="s">
         <v>280</v>
@@ -8144,7 +8144,7 @@
         <v>16</v>
       </c>
       <c r="L263" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M263" s="0" t="s">
         <v>280</v>
@@ -8164,7 +8164,7 @@
         <v>16</v>
       </c>
       <c r="L264" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M264" s="0" t="s">
         <v>280</v>
@@ -8184,7 +8184,7 @@
         <v>16</v>
       </c>
       <c r="L265" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M265" s="0" t="s">
         <v>280</v>
@@ -8204,7 +8204,7 @@
         <v>16</v>
       </c>
       <c r="L266" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M266" s="0" t="s">
         <v>280</v>
@@ -8224,7 +8224,7 @@
         <v>16</v>
       </c>
       <c r="L267" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M267" s="0" t="s">
         <v>796</v>
@@ -8244,7 +8244,7 @@
         <v>16</v>
       </c>
       <c r="L268" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M268" s="0" t="s">
         <v>240</v>
@@ -8264,7 +8264,7 @@
         <v>16</v>
       </c>
       <c r="L269" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M269" s="0" t="s">
         <v>42</v>
@@ -8284,7 +8284,7 @@
         <v>16</v>
       </c>
       <c r="L270" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M270" s="0" t="s">
         <v>42</v>
@@ -8304,7 +8304,7 @@
         <v>16</v>
       </c>
       <c r="L271" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M271" s="0" t="s">
         <v>154</v>
@@ -8324,7 +8324,7 @@
         <v>16</v>
       </c>
       <c r="L272" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M272" s="0" t="s">
         <v>162</v>
@@ -8344,7 +8344,7 @@
         <v>16</v>
       </c>
       <c r="L273" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M273" s="0" t="n">
         <v>0.001</v>
@@ -8364,7 +8364,7 @@
         <v>16</v>
       </c>
       <c r="L274" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M274" s="0" t="s">
         <v>154</v>
@@ -8384,7 +8384,7 @@
         <v>16</v>
       </c>
       <c r="L275" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M275" s="0" t="s">
         <v>711</v>
@@ -8404,7 +8404,7 @@
         <v>16</v>
       </c>
       <c r="L276" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M276" s="0" t="s">
         <v>796</v>
@@ -8424,7 +8424,7 @@
         <v>16</v>
       </c>
       <c r="L277" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M277" s="0" t="s">
         <v>154</v>
@@ -8444,7 +8444,7 @@
         <v>16</v>
       </c>
       <c r="L278" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M278" s="0" t="s">
         <v>42</v>
@@ -8464,7 +8464,7 @@
         <v>16</v>
       </c>
       <c r="L279" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M279" s="0" t="s">
         <v>330</v>
@@ -8484,7 +8484,7 @@
         <v>16</v>
       </c>
       <c r="L280" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M280" s="0" t="s">
         <v>704</v>
@@ -8504,7 +8504,7 @@
         <v>16</v>
       </c>
       <c r="L281" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M281" s="0" t="s">
         <v>704</v>
@@ -8524,7 +8524,7 @@
         <v>16</v>
       </c>
       <c r="L282" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M282" s="0" t="s">
         <v>280</v>
@@ -8544,7 +8544,7 @@
         <v>16</v>
       </c>
       <c r="L283" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M283" s="0" t="s">
         <v>280</v>
@@ -8564,7 +8564,7 @@
         <v>16</v>
       </c>
       <c r="L284" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M284" s="0" t="s">
         <v>280</v>
@@ -8584,7 +8584,7 @@
         <v>16</v>
       </c>
       <c r="L285" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M285" s="0" t="s">
         <v>280</v>
@@ -8604,7 +8604,7 @@
         <v>16</v>
       </c>
       <c r="L286" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M286" s="0" t="s">
         <v>854</v>
@@ -8624,7 +8624,7 @@
         <v>16</v>
       </c>
       <c r="L287" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M287" s="0" t="s">
         <v>854</v>
@@ -8644,7 +8644,7 @@
         <v>16</v>
       </c>
       <c r="L288" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M288" s="0" t="s">
         <v>854</v>
@@ -8664,7 +8664,7 @@
         <v>16</v>
       </c>
       <c r="L289" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M289" s="0" t="s">
         <v>42</v>
@@ -8684,7 +8684,7 @@
         <v>16</v>
       </c>
       <c r="L290" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M290" s="0" t="n">
         <v>1</v>
@@ -8704,7 +8704,7 @@
         <v>16</v>
       </c>
       <c r="L291" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M291" s="0" t="s">
         <v>330</v>
@@ -8724,7 +8724,7 @@
         <v>16</v>
       </c>
       <c r="L292" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M292" s="0" t="s">
         <v>330</v>
@@ -8744,7 +8744,7 @@
         <v>16</v>
       </c>
       <c r="L293" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M293" s="0" t="s">
         <v>42</v>
@@ -8764,7 +8764,7 @@
         <v>16</v>
       </c>
       <c r="L294" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M294" s="0" t="s">
         <v>879</v>
@@ -8784,7 +8784,7 @@
         <v>16</v>
       </c>
       <c r="L295" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M295" s="0" t="s">
         <v>879</v>
@@ -8804,7 +8804,7 @@
         <v>16</v>
       </c>
       <c r="L296" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M296" s="0" t="s">
         <v>76</v>
@@ -8824,7 +8824,7 @@
         <v>16</v>
       </c>
       <c r="L297" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M297" s="0" t="s">
         <v>76</v>
@@ -8844,7 +8844,7 @@
         <v>16</v>
       </c>
       <c r="L298" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M298" s="0" t="s">
         <v>76</v>
@@ -8864,7 +8864,7 @@
         <v>16</v>
       </c>
       <c r="L299" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M299" s="0" t="s">
         <v>76</v>
@@ -8884,7 +8884,7 @@
         <v>16</v>
       </c>
       <c r="L300" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M300" s="0" t="s">
         <v>76</v>
@@ -8904,7 +8904,7 @@
         <v>16</v>
       </c>
       <c r="L301" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="M301" s="0" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Fix a mistake where an inpoc and intpcalcite field were interchanged when adding intpoc in pre nemo file #813.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -1603,16 +1603,16 @@
     <t xml:space="preserve">intpcalcite</t>
   </si>
   <si>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P1 (mol m-2 s-1) tendency_of_ocean_mole_content_of_calcite_expressed_as_carbon_due_to_biological_production : Vertically integrated calcite production </t>
+  </si>
+  <si>
+    <t xml:space="preserve">intpoc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P1 (mol m-2 s-1) tendency_of_ocean_mole_content_of_calcite_expressed_as_carbon_due_to_biological_production : Vertically integrated calcite production </t>
-  </si>
-  <si>
-    <t xml:space="preserve">intpoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPCAL</t>
   </si>
   <si>
     <t xml:space="preserve"> P2 (kg m-2) ocean_mass_content_of_particulate_organic_matter_expressed_as_carbon : Vertically integrated POC</t>
@@ -2736,7 +2736,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2766,12 +2766,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2829,7 +2823,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2852,11 +2846,11 @@
   </sheetPr>
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="219:219"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H174" activeCellId="0" sqref="H174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -6418,7 +6412,7 @@
         <v>538</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I177" s="0" t="s">
         <v>16</v>

</xml_diff>